<commit_message>
conditional formatting number format ignored bug
</commit_message>
<xml_diff>
--- a/src/main/resources/simple-invoice.xlsx
+++ b/src/main/resources/simple-invoice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GregWoolsey\git\sheet-tables\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C806154-DDC7-4959-A828-DC6BC229D98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A6B6A4-33A7-4128-A3C2-32DFBD0C7D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33375" yWindow="11820" windowWidth="28845" windowHeight="17265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="630" windowWidth="30060" windowHeight="23370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="187">
   <si>
     <t>Demo Ltd</t>
   </si>
@@ -593,6 +593,12 @@
   <si>
     <t>(no filters enabled)</t>
   </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
 </sst>
 </file>
 
@@ -601,7 +607,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -613,35 +619,48 @@
       <sz val="20"/>
       <color theme="1"/>
       <name val="Open Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Open Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Open Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Open Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -697,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -726,11 +745,22 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -761,9 +791,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="3"/>
-      <tableStyleElement type="firstRowStripe" dxfId="2"/>
-      <tableStyleElement type="secondRowStripe" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="6"/>
+      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+      <tableStyleElement type="secondRowStripe" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -775,6 +805,1185 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.2692038495188102E-2"/>
+          <c:y val="2.5428331875182269E-2"/>
+          <c:w val="0.90286351706036749"/>
+          <c:h val="0.43676509186351709"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Length</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet2!$A$7:$D$58</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Sheet2!$A$7:$A$58</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet2!$A$7:$A$58</c:f>
+              <c:strCache>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>Alabama</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Alaska</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Arizona</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Arkansas</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>California</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Colorado</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Connecticut</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Delaware</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>District of Columbia</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Florida</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Georgia</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Hawaii</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Idaho</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Illinois</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Indiana</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Iowa</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Kansas</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Kentucky</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Louisiana</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Maine</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Maryland</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Massachusetts</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Michigan</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Minnesota</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Mississippi</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Missouri</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Montana</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Nebraska</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Nevada</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>New Hampshire</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>New Jersey</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>New Mexico</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>New York</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>North Carolina</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>North Dakota</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Ohio</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Oklahoma</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Oregon</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Pennsylvania</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Puerto Rico</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Rhode Island</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>South Carolina</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>South Dakota</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Tennessee</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Texas</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Utah</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Vermont</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>Virginia</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>Washington</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>West Virginia</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>Wisconsin</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>Wyoming</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$7:$E$58</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-383A-4225-B3BF-BD314A09652C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1362194159"/>
+        <c:axId val="1355308159"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1362194159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1355308159"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1355308159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1362194159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BD47571-BF4E-6081-E2C4-BC0E01A3E8F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -790,12 +1999,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{795BA97F-645C-4425-8945-AE2CD9558FAC}" name="Table2" displayName="Table2" ref="B6:D58" totalsRowShown="0">
-  <autoFilter ref="B6:D58" xr:uid="{795BA97F-645C-4425-8945-AE2CD9558FAC}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{795BA97F-645C-4425-8945-AE2CD9558FAC}" name="Table2" displayName="Table2" ref="A6:E58" totalsRowShown="0">
+  <autoFilter ref="A6:E58" xr:uid="{795BA97F-645C-4425-8945-AE2CD9558FAC}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{F34889A9-CB70-4A7A-AB1B-C7EA25F3C362}" name="State"/>
-    <tableColumn id="2" xr3:uid="{E70045C6-767A-43D6-8BB0-654B117BDFC1}" name="Number" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{E70045C6-767A-43D6-8BB0-654B117BDFC1}" name="Number" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{EF8CFBBA-F465-4B36-8BEF-09918AB53AC2}" name="Code"/>
+    <tableColumn id="4" xr3:uid="{86275F93-EEF5-4A42-B6C5-142AB4F62F65}" name="Alpha" dataDxfId="2">
+      <calculatedColumnFormula>LEFT(Table2[[#This Row],[Code]],1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{02FD46AE-D188-4146-847E-0E35DA4CDF22}" name="Length" dataDxfId="0">
+      <calculatedColumnFormula>LEN(Table2[[#This Row],[State]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -29163,609 +30378,1038 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B92B6B-2EB1-4571-992D-CE294756552B}">
-  <dimension ref="A2:D58"/>
+  <dimension ref="A2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.125" customWidth="1"/>
+    <col min="2" max="2" width="9.125" customWidth="1"/>
+    <col min="5" max="5" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s">
         <v>180</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="D6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="D7" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>A</v>
+      </c>
+      <c r="E7" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="D8" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>A</v>
+      </c>
+      <c r="E8" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="D9" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>A</v>
+      </c>
+      <c r="E9" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="D10" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>A</v>
+      </c>
+      <c r="E10" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="D11" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>C</v>
+      </c>
+      <c r="E11" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="D12" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>C</v>
+      </c>
+      <c r="E12" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="B13" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="D13" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>C</v>
+      </c>
+      <c r="E13" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="D14" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>D</v>
+      </c>
+      <c r="E14" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="B15" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="D15" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>D</v>
+      </c>
+      <c r="E15" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="D16" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>F</v>
+      </c>
+      <c r="E16" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="B17" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="D17" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>G</v>
+      </c>
+      <c r="E17" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="B18" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="D18" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>H</v>
+      </c>
+      <c r="E18" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C19" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="D19" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>I</v>
+      </c>
+      <c r="E19" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="D20" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>I</v>
+      </c>
+      <c r="E20" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="D21" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>I</v>
+      </c>
+      <c r="E21" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="D22" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>I</v>
+      </c>
+      <c r="E22" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="B23" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C23" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="D23" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>K</v>
+      </c>
+      <c r="E23" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="B24" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C24" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="D24" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>K</v>
+      </c>
+      <c r="E24" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="B25" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C25" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="D25" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>L</v>
+      </c>
+      <c r="E25" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="B26" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C26" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="D26" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>M</v>
+      </c>
+      <c r="E26" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="B27" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C27" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="D27" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>M</v>
+      </c>
+      <c r="E27" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="B28" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C28" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="D28" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>M</v>
+      </c>
+      <c r="E28" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="B29" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C29" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="D29" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>M</v>
+      </c>
+      <c r="E29" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="B30" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C30" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="D30" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>M</v>
+      </c>
+      <c r="E30" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="B31" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="D31" t="s">
+      <c r="C31" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="D31" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>M</v>
+      </c>
+      <c r="E31" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="B32" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="D32" t="s">
+      <c r="C32" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="D32" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>M</v>
+      </c>
+      <c r="E32" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="B33" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D33" t="s">
+      <c r="C33" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="D33" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>M</v>
+      </c>
+      <c r="E33" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="B34" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="D34" t="s">
+      <c r="C34" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="D34" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>N</v>
+      </c>
+      <c r="E34" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="B35" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="D35" t="s">
+      <c r="C35" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="D35" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>N</v>
+      </c>
+      <c r="E35" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>111</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="B36" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D36" t="s">
+      <c r="C36" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="D36" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>N</v>
+      </c>
+      <c r="E36" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>114</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="B37" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="D37" t="s">
+      <c r="C37" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="D37" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>N</v>
+      </c>
+      <c r="E37" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="B38" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="D38" t="s">
+      <c r="C38" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="D38" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>N</v>
+      </c>
+      <c r="E38" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>120</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="B39" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="D39" t="s">
+      <c r="C39" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="D39" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>N</v>
+      </c>
+      <c r="E39" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>123</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="B40" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D40" t="s">
+      <c r="C40" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="D40" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>N</v>
+      </c>
+      <c r="E40" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="B41" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="D41" t="s">
+      <c r="C41" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="D41" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>N</v>
+      </c>
+      <c r="E41" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>129</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="B42" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="D42" t="s">
+      <c r="C42" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="D42" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>O</v>
+      </c>
+      <c r="E42" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>132</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="B43" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="D43" t="s">
+      <c r="C43" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="D43" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>O</v>
+      </c>
+      <c r="E43" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>135</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="B44" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="D44" t="s">
+      <c r="C44" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="D44" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>O</v>
+      </c>
+      <c r="E44" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="B45" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="D45" t="s">
+      <c r="C45" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="D45" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>P</v>
+      </c>
+      <c r="E45" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>141</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="B46" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="D46" t="s">
+      <c r="C46" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="D46" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>P</v>
+      </c>
+      <c r="E46" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>144</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="B47" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D47" t="s">
+      <c r="C47" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+      <c r="D47" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>R</v>
+      </c>
+      <c r="E47" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>147</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="B48" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="D48" t="s">
+      <c r="C48" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+      <c r="D48" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>S</v>
+      </c>
+      <c r="E48" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>150</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="B49" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="D49" t="s">
+      <c r="C49" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+      <c r="D49" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>S</v>
+      </c>
+      <c r="E49" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>153</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="B50" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="D50" t="s">
+      <c r="C50" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+      <c r="D50" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>T</v>
+      </c>
+      <c r="E50" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="B51" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="D51" t="s">
+      <c r="C51" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+      <c r="D51" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>T</v>
+      </c>
+      <c r="E51" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>159</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="B52" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="D52" t="s">
+      <c r="C52" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="D52" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>U</v>
+      </c>
+      <c r="E52" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>162</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="B53" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="D53" t="s">
+      <c r="C53" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="D53" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>V</v>
+      </c>
+      <c r="E53" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>165</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="B54" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="D54" t="s">
+      <c r="C54" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="D54" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>V</v>
+      </c>
+      <c r="E54" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>168</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="B55" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="D55" t="s">
+      <c r="C55" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+      <c r="D55" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>W</v>
+      </c>
+      <c r="E55" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>171</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="B56" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="D56" t="s">
+      <c r="C56" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+      <c r="D56" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>W</v>
+      </c>
+      <c r="E56" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>174</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="B57" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="D57" t="s">
+      <c r="C57" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="D57" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>W</v>
+      </c>
+      <c r="E57" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>177</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="B58" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="D58" t="s">
+      <c r="C58" t="s">
         <v>179</v>
       </c>
+      <c r="D58" t="str">
+        <f>LEFT(Table2[[#This Row],[Code]],1)</f>
+        <v>W</v>
+      </c>
+      <c r="E58" s="19">
+        <f>LEN(Table2[[#This Row],[State]])</f>
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E7:E58">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>